<commit_message>
styling update for mobile
</commit_message>
<xml_diff>
--- a/shows.xlsx
+++ b/shows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\Projects\indigo-radio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87764B5-8F3C-43F0-86CE-DE93E7EC3F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE157AE1-E963-4321-9FF5-40918DDA6DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{03067A53-B422-40DC-88F7-7DF185341E14}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{03067A53-B422-40DC-88F7-7DF185341E14}"/>
   </bookViews>
   <sheets>
     <sheet name="shows" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>https://i0.wp.com/indigofmradio.com/wp-content/uploads/2021/12/asleep-at-the-wheel.jpg</t>
+  </si>
+  <si>
+    <t>playlist-tue-12pm</t>
+  </si>
+  <si>
+    <t>Playlist</t>
   </si>
 </sst>
 </file>
@@ -743,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A9F77F-769A-491E-840B-1A8CA0C8AE6D}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,6 +1240,35 @@
         <v>98</v>
       </c>
     </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" t="s">
+        <v>97</v>
+      </c>
+      <c r="O18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R18" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>